<commit_message>
2 dic 2025 initial tests until Ga laptop panicked and did no more
</commit_message>
<xml_diff>
--- a/Datasets/II Semester 2025/Results - Final Sensors.xlsx
+++ b/Datasets/II Semester 2025/Results - Final Sensors.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Daniel Quesada\Documents\GitHub\eWave\Datasets\II Semester 2025\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Gabu\Documents\GitHub\eWave\Datasets\II Semester 2025\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{10258E38-17D6-4DC3-8E86-4EBDBBE45DB2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3480B27B-7A41-45D1-A8F6-4600C372759B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{067E96B3-EB7F-4CEE-B660-BBE446B0B978}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" activeTab="1" xr2:uid="{067E96B3-EB7F-4CEE-B660-BBE446B0B978}"/>
   </bookViews>
   <sheets>
     <sheet name="Results" sheetId="7" r:id="rId1"/>
@@ -621,7 +621,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -632,17 +632,16 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1071,17 +1070,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BCB99CC0-1677-490B-A944-764B00B51635}">
   <dimension ref="A1:L44"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView topLeftCell="A37" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="2" width="10.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="2" width="10.7109375" bestFit="1" customWidth="1"/>
     <col min="3" max="10" width="12" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="12.7109375" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="12" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>3</v>
       </c>
@@ -1119,11 +1118,11 @@
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>10</v>
       </c>
-      <c r="B2" s="5" t="s">
+      <c r="B2" t="s">
         <v>20</v>
       </c>
       <c r="C2">
@@ -1157,11 +1156,11 @@
         <v>0.99425987498663038</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>10</v>
       </c>
-      <c r="B3" s="5" t="s">
+      <c r="B3" t="s">
         <v>19</v>
       </c>
       <c r="C3">
@@ -1195,11 +1194,11 @@
         <v>1.4319671505134792</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>10</v>
       </c>
-      <c r="B4" s="5" t="s">
+      <c r="B4" t="s">
         <v>18</v>
       </c>
       <c r="C4">
@@ -1233,11 +1232,11 @@
         <v>0.66323567967107411</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>10</v>
       </c>
-      <c r="B5" s="5" t="s">
+      <c r="B5" t="s">
         <v>17</v>
       </c>
       <c r="C5">
@@ -1271,11 +1270,11 @@
         <v>0.47407032379900588</v>
       </c>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>10</v>
       </c>
-      <c r="B6" s="5" t="s">
+      <c r="B6" t="s">
         <v>16</v>
       </c>
       <c r="C6">
@@ -1309,11 +1308,11 @@
         <v>0.5133271289803476</v>
       </c>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>10</v>
       </c>
-      <c r="B7" s="5" t="s">
+      <c r="B7" t="s">
         <v>21</v>
       </c>
       <c r="C7">
@@ -1347,11 +1346,11 @@
         <v>0.6844931801537899</v>
       </c>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>12.5</v>
       </c>
-      <c r="B8" s="5" t="s">
+      <c r="B8" t="s">
         <v>20</v>
       </c>
       <c r="C8">
@@ -1385,11 +1384,11 @@
         <v>0.87438816285499354</v>
       </c>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>12.5</v>
       </c>
-      <c r="B9" s="5" t="s">
+      <c r="B9" t="s">
         <v>19</v>
       </c>
       <c r="C9">
@@ -1423,11 +1422,11 @@
         <v>0.97016321646400394</v>
       </c>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>12.5</v>
       </c>
-      <c r="B10" s="5" t="s">
+      <c r="B10" t="s">
         <v>18</v>
       </c>
       <c r="C10">
@@ -1461,11 +1460,11 @@
         <v>0.47393507147560848</v>
       </c>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>12.5</v>
       </c>
-      <c r="B11" s="5" t="s">
+      <c r="B11" t="s">
         <v>17</v>
       </c>
       <c r="C11">
@@ -1499,11 +1498,11 @@
         <v>0.40839657223935699</v>
       </c>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>12.5</v>
       </c>
-      <c r="B12" s="5" t="s">
+      <c r="B12" t="s">
         <v>16</v>
       </c>
       <c r="C12">
@@ -1537,11 +1536,11 @@
         <v>0.31671180782006297</v>
       </c>
     </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>12.5</v>
       </c>
-      <c r="B13" s="5" t="s">
+      <c r="B13" t="s">
         <v>21</v>
       </c>
       <c r="C13">
@@ -1575,11 +1574,11 @@
         <v>3.5125360773263368</v>
       </c>
     </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>15</v>
       </c>
-      <c r="B14" s="5" t="s">
+      <c r="B14" t="s">
         <v>20</v>
       </c>
       <c r="C14">
@@ -1613,11 +1612,11 @@
         <v>0.82184594716369452</v>
       </c>
     </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>15</v>
       </c>
-      <c r="B15" s="5" t="s">
+      <c r="B15" t="s">
         <v>19</v>
       </c>
       <c r="C15">
@@ -1651,11 +1650,11 @@
         <v>1.6928101718428381</v>
       </c>
     </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>15</v>
       </c>
-      <c r="B16" s="5" t="s">
+      <c r="B16" t="s">
         <v>18</v>
       </c>
       <c r="C16">
@@ -1689,11 +1688,11 @@
         <v>0.34912820593784621</v>
       </c>
     </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>15</v>
       </c>
-      <c r="B17" s="5" t="s">
+      <c r="B17" t="s">
         <v>17</v>
       </c>
       <c r="C17">
@@ -1727,11 +1726,11 @@
         <v>1.5829223306549818</v>
       </c>
     </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>15</v>
       </c>
-      <c r="B18" s="5" t="s">
+      <c r="B18" t="s">
         <v>16</v>
       </c>
       <c r="C18">
@@ -1765,11 +1764,11 @@
         <v>0.37239715416958513</v>
       </c>
     </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>15</v>
       </c>
-      <c r="B19" s="5" t="s">
+      <c r="B19" t="s">
         <v>21</v>
       </c>
       <c r="C19">
@@ -1803,11 +1802,11 @@
         <v>0.35146794438723039</v>
       </c>
     </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>17.5</v>
       </c>
-      <c r="B20" s="5" t="s">
+      <c r="B20" t="s">
         <v>20</v>
       </c>
       <c r="C20">
@@ -1841,11 +1840,11 @@
         <v>0.13674233014607934</v>
       </c>
     </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>17.5</v>
       </c>
-      <c r="B21" s="5" t="s">
+      <c r="B21" t="s">
         <v>20</v>
       </c>
       <c r="C21">
@@ -1879,11 +1878,11 @@
         <v>0.20482425169301452</v>
       </c>
     </row>
-    <row r="22" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>17.5</v>
       </c>
-      <c r="B22" s="5" t="s">
+      <c r="B22" t="s">
         <v>20</v>
       </c>
       <c r="C22">
@@ -1917,11 +1916,11 @@
         <v>0.1491713097669646</v>
       </c>
     </row>
-    <row r="23" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>17.5</v>
       </c>
-      <c r="B23" s="5" t="s">
+      <c r="B23" t="s">
         <v>22</v>
       </c>
       <c r="C23">
@@ -1955,11 +1954,11 @@
         <v>0.12632450906248469</v>
       </c>
     </row>
-    <row r="24" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>17.5</v>
       </c>
-      <c r="B24" s="5" t="s">
+      <c r="B24" t="s">
         <v>19</v>
       </c>
       <c r="C24">
@@ -1993,11 +1992,11 @@
         <v>0.17693363368686973</v>
       </c>
     </row>
-    <row r="25" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>17.5</v>
       </c>
-      <c r="B25" s="5" t="s">
+      <c r="B25" t="s">
         <v>18</v>
       </c>
       <c r="C25">
@@ -2031,11 +2030,11 @@
         <v>0.14438635662454116</v>
       </c>
     </row>
-    <row r="26" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>17.5</v>
       </c>
-      <c r="B26" s="5" t="s">
+      <c r="B26" t="s">
         <v>17</v>
       </c>
       <c r="C26">
@@ -2069,11 +2068,11 @@
         <v>0.12280022592880278</v>
       </c>
     </row>
-    <row r="27" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>17.5</v>
       </c>
-      <c r="B27" s="5" t="s">
+      <c r="B27" t="s">
         <v>16</v>
       </c>
       <c r="C27">
@@ -2107,11 +2106,11 @@
         <v>0.12948272793337412</v>
       </c>
     </row>
-    <row r="28" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>17.5</v>
       </c>
-      <c r="B28" s="5" t="s">
+      <c r="B28" t="s">
         <v>21</v>
       </c>
       <c r="C28">
@@ -2145,11 +2144,11 @@
         <v>0.23592606876244379</v>
       </c>
     </row>
-    <row r="29" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>20</v>
       </c>
-      <c r="B29" s="5" t="s">
+      <c r="B29" t="s">
         <v>20</v>
       </c>
       <c r="C29">
@@ -2183,11 +2182,11 @@
         <v>0.11433157394113133</v>
       </c>
     </row>
-    <row r="30" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>20</v>
       </c>
-      <c r="B30" s="5" t="s">
+      <c r="B30" t="s">
         <v>19</v>
       </c>
       <c r="C30">
@@ -2221,11 +2220,11 @@
         <v>3.2960139589624524</v>
       </c>
     </row>
-    <row r="31" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>20</v>
       </c>
-      <c r="B31" s="5" t="s">
+      <c r="B31" t="s">
         <v>18</v>
       </c>
       <c r="C31">
@@ -2259,11 +2258,11 @@
         <v>0.75003182789538847</v>
       </c>
     </row>
-    <row r="32" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>20</v>
       </c>
-      <c r="B32" s="5" t="s">
+      <c r="B32" t="s">
         <v>17</v>
       </c>
       <c r="C32">
@@ -2297,11 +2296,11 @@
         <v>0.14125049962792813</v>
       </c>
     </row>
-    <row r="33" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>20</v>
       </c>
-      <c r="B33" s="5" t="s">
+      <c r="B33" t="s">
         <v>16</v>
       </c>
       <c r="C33">
@@ -2335,11 +2334,11 @@
         <v>0.22937602714105437</v>
       </c>
     </row>
-    <row r="34" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>20</v>
       </c>
-      <c r="B34" s="5" t="s">
+      <c r="B34" t="s">
         <v>21</v>
       </c>
       <c r="C34">
@@ -2373,11 +2372,11 @@
         <v>0.16958907352221608</v>
       </c>
     </row>
-    <row r="35" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>22.5</v>
       </c>
-      <c r="B35" s="5" t="s">
+      <c r="B35" t="s">
         <v>20</v>
       </c>
       <c r="C35">
@@ -2411,11 +2410,11 @@
         <v>3.6844287035645795</v>
       </c>
     </row>
-    <row r="36" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A36">
         <v>22.5</v>
       </c>
-      <c r="B36" s="5" t="s">
+      <c r="B36" t="s">
         <v>19</v>
       </c>
       <c r="C36">
@@ -2449,11 +2448,11 @@
         <v>6.7292167108884596E-2</v>
       </c>
     </row>
-    <row r="37" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A37">
         <v>22.5</v>
       </c>
-      <c r="B37" s="5" t="s">
+      <c r="B37" t="s">
         <v>18</v>
       </c>
       <c r="C37">
@@ -2487,11 +2486,11 @@
         <v>8.6431833496537824E-2</v>
       </c>
     </row>
-    <row r="38" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A38">
         <v>22.5</v>
       </c>
-      <c r="B38" s="5" t="s">
+      <c r="B38" t="s">
         <v>17</v>
       </c>
       <c r="C38">
@@ -2525,11 +2524,11 @@
         <v>0.38469166346338279</v>
       </c>
     </row>
-    <row r="39" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A39">
         <v>22.5</v>
       </c>
-      <c r="B39" s="5" t="s">
+      <c r="B39" t="s">
         <v>16</v>
       </c>
       <c r="C39">
@@ -2563,11 +2562,11 @@
         <v>0.15923270965237604</v>
       </c>
     </row>
-    <row r="40" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A40">
         <v>22.5</v>
       </c>
-      <c r="B40" s="5" t="s">
+      <c r="B40" t="s">
         <v>21</v>
       </c>
       <c r="C40">
@@ -2601,11 +2600,11 @@
         <v>0.1071048974888421</v>
       </c>
     </row>
-    <row r="41" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A41">
         <v>25</v>
       </c>
-      <c r="B41" s="5" t="s">
+      <c r="B41" t="s">
         <v>21</v>
       </c>
       <c r="C41">
@@ -2639,11 +2638,11 @@
         <v>6.2846332685778508E-2</v>
       </c>
     </row>
-    <row r="42" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A42">
         <v>27.5</v>
       </c>
-      <c r="B42" s="5" t="s">
+      <c r="B42" t="s">
         <v>21</v>
       </c>
       <c r="C42">
@@ -2677,11 +2676,11 @@
         <v>0.14173594591965136</v>
       </c>
     </row>
-    <row r="43" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A43">
         <v>30</v>
       </c>
-      <c r="B43" s="5" t="s">
+      <c r="B43" t="s">
         <v>21</v>
       </c>
       <c r="C43">
@@ -2715,8 +2714,8 @@
         <v>0.49885142281930339</v>
       </c>
     </row>
-    <row r="44" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="B44" s="5" t="s">
+    <row r="44" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B44" t="s">
         <v>15</v>
       </c>
     </row>
@@ -2730,34 +2729,38 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8B065C34-D71F-4F02-8C1B-51E36B9B764A}">
-  <dimension ref="B2:L9"/>
+  <dimension ref="B1:M9"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I5" sqref="I5"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="2.6640625" customWidth="1"/>
-    <col min="2" max="3" width="11.109375" customWidth="1"/>
-    <col min="4" max="5" width="9.5546875" bestFit="1" customWidth="1"/>
-    <col min="6" max="8" width="10.5546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="2.7109375" customWidth="1"/>
+    <col min="2" max="3" width="11.140625" customWidth="1"/>
+    <col min="4" max="5" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="6" max="8" width="10.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:12" x14ac:dyDescent="0.3">
+    <row r="1" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="L1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B2" s="3"/>
-      <c r="C2" s="8" t="s">
+      <c r="C2" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="D2" s="8"/>
-      <c r="E2" s="8"/>
-      <c r="F2" s="8"/>
-      <c r="G2" s="8"/>
-      <c r="H2" s="8"/>
-      <c r="I2" s="8"/>
-      <c r="L2" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="3" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="D2" s="6"/>
+      <c r="E2" s="6"/>
+      <c r="F2" s="6"/>
+      <c r="G2" s="6"/>
+      <c r="H2" s="6"/>
+      <c r="I2" s="6"/>
+    </row>
+    <row r="3" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B3" s="1" t="s">
         <v>1</v>
       </c>
@@ -2785,160 +2788,181 @@
       <c r="J3" s="1">
         <v>27.5</v>
       </c>
-    </row>
-    <row r="4" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="K3" s="1">
+        <v>30</v>
+      </c>
+      <c r="L3" s="1">
+        <v>32.5</v>
+      </c>
+      <c r="M3" s="1">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="4" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B4" s="3">
         <v>90</v>
       </c>
-      <c r="C4" s="6">
+      <c r="C4" s="4">
         <v>25.943822784810127</v>
       </c>
-      <c r="D4" s="6">
+      <c r="D4" s="4">
         <v>17.605999999999998</v>
       </c>
-      <c r="E4" s="6">
+      <c r="E4" s="4">
         <v>41.455898734177197</v>
       </c>
-      <c r="F4" s="6">
+      <c r="F4" s="4">
         <v>48.408075949367088</v>
       </c>
-      <c r="G4" s="6">
+      <c r="G4" s="4">
         <v>61.213670886075953</v>
       </c>
-      <c r="H4" s="6">
+      <c r="H4" s="4">
         <v>49.597924050632912</v>
       </c>
-      <c r="I4" s="6">
+      <c r="I4" s="4">
         <v>73.941189873417727</v>
       </c>
-      <c r="J4" s="6">
+      <c r="J4" s="4">
         <v>101.45691139240506</v>
       </c>
-    </row>
-    <row r="5" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="K4" s="4">
+        <v>65.3</v>
+      </c>
+      <c r="L4" s="4">
+        <v>84.49</v>
+      </c>
+      <c r="M4" s="4">
+        <v>107.52</v>
+      </c>
+    </row>
+    <row r="5" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B5" s="3">
         <v>120</v>
       </c>
-      <c r="C5" s="6">
+      <c r="C5" s="4">
         <v>30.072126582278482</v>
       </c>
-      <c r="D5" s="6">
+      <c r="D5" s="4">
         <v>22.845848101265823</v>
       </c>
-      <c r="E5" s="6">
+      <c r="E5" s="4">
         <v>54.199518987341769</v>
       </c>
-      <c r="F5" s="6">
+      <c r="F5" s="4">
         <v>58.283037974683545</v>
       </c>
-      <c r="G5" s="6">
+      <c r="G5" s="4">
         <v>73.502784810126585</v>
       </c>
-      <c r="H5" s="6">
+      <c r="H5" s="4">
         <v>61.142962025316457</v>
       </c>
-      <c r="I5" s="6"/>
-      <c r="J5" s="6"/>
-    </row>
-    <row r="6" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="I5" s="4"/>
+      <c r="J5" s="4"/>
+    </row>
+    <row r="6" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B6" s="3">
         <v>150</v>
       </c>
-      <c r="C6" s="6">
+      <c r="C6" s="4">
         <v>34.224962025316458</v>
       </c>
-      <c r="D6" s="6">
+      <c r="D6" s="4">
         <v>26.487392405063289</v>
       </c>
-      <c r="E6" s="6">
+      <c r="E6" s="4">
         <v>59.902506329113898</v>
       </c>
-      <c r="F6" s="6">
+      <c r="F6" s="4">
         <v>70.313291139240505</v>
       </c>
-      <c r="G6" s="6">
+      <c r="G6" s="4">
         <v>85.81311392405064</v>
       </c>
-      <c r="H6" s="6">
+      <c r="H6" s="4">
         <v>75.606683544303792</v>
       </c>
-      <c r="I6" s="6"/>
-      <c r="J6" s="6"/>
-    </row>
-    <row r="7" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="I6" s="4"/>
+      <c r="J6" s="4"/>
+    </row>
+    <row r="7" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B7" s="3">
         <v>180</v>
       </c>
-      <c r="C7" s="6">
+      <c r="C7" s="4">
         <v>38.721620253164559</v>
       </c>
-      <c r="D7" s="6">
+      <c r="D7" s="4">
         <v>31.635696202531648</v>
       </c>
-      <c r="E7" s="6">
+      <c r="E7" s="4">
         <v>74.032506329113929</v>
       </c>
-      <c r="F7" s="6">
+      <c r="F7" s="4">
         <v>82.847240506329115</v>
       </c>
-      <c r="G7" s="6">
+      <c r="G7" s="4">
         <v>98.923815789473679</v>
       </c>
-      <c r="H7" s="6">
+      <c r="H7" s="4">
         <v>87.952253164556964</v>
       </c>
-      <c r="I7" s="6"/>
-      <c r="J7" s="6"/>
-    </row>
-    <row r="8" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="I7" s="4"/>
+      <c r="J7" s="4"/>
+    </row>
+    <row r="8" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B8" s="3">
         <v>210</v>
       </c>
-      <c r="C8" s="6">
+      <c r="C8" s="4">
         <v>40.373797468354432</v>
       </c>
-      <c r="D8" s="6">
+      <c r="D8" s="4">
         <v>34.37341772151899</v>
       </c>
-      <c r="E8" s="6">
+      <c r="E8" s="4">
         <v>79.921772151898693</v>
       </c>
-      <c r="F8" s="6">
+      <c r="F8" s="4">
         <v>94.448227848101268</v>
       </c>
-      <c r="G8" s="6">
+      <c r="G8" s="4">
         <v>114.66673417721519</v>
       </c>
-      <c r="H8" s="6">
+      <c r="H8" s="4">
         <v>99.898253164556962</v>
       </c>
-      <c r="I8" s="6"/>
-      <c r="J8" s="6"/>
-    </row>
-    <row r="9" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="I8" s="4"/>
+      <c r="J8" s="4"/>
+    </row>
+    <row r="9" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B9" s="2">
         <v>240</v>
       </c>
-      <c r="C9" s="7">
+      <c r="C9" s="5">
         <v>44.132936708860761</v>
       </c>
-      <c r="D9" s="7">
+      <c r="D9" s="5">
         <v>40.320101265822785</v>
       </c>
-      <c r="E9" s="7">
+      <c r="E9" s="5">
         <v>89.431051282051286</v>
       </c>
-      <c r="F9" s="7">
+      <c r="F9" s="5">
         <v>107.3167341772152</v>
       </c>
-      <c r="G9" s="7">
+      <c r="G9" s="5">
         <v>131.08458227848101</v>
       </c>
-      <c r="H9" s="7">
+      <c r="H9" s="5">
         <v>126.13407594936709</v>
       </c>
-      <c r="I9" s="7"/>
-      <c r="J9" s="7"/>
+      <c r="I9" s="5"/>
+      <c r="J9" s="5"/>
+      <c r="K9" s="5"/>
+      <c r="L9" s="5"/>
+      <c r="M9" s="5"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -2954,27 +2978,27 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="2.6640625" customWidth="1"/>
-    <col min="2" max="3" width="11.109375" customWidth="1"/>
+    <col min="1" max="1" width="2.7109375" customWidth="1"/>
+    <col min="2" max="3" width="11.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="2" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B2" s="3"/>
-      <c r="C2" s="4" t="s">
+      <c r="C2" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="D2" s="4"/>
-      <c r="E2" s="4"/>
-      <c r="F2" s="4"/>
-      <c r="G2" s="4"/>
-      <c r="H2" s="4"/>
+      <c r="D2" s="7"/>
+      <c r="E2" s="7"/>
+      <c r="F2" s="7"/>
+      <c r="G2" s="7"/>
+      <c r="H2" s="7"/>
       <c r="J2" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="3" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B3" s="1" t="s">
         <v>1</v>
       </c>
@@ -2997,7 +3021,7 @@
         <v>22.5</v>
       </c>
     </row>
-    <row r="4" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="4" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B4" s="3">
         <v>90</v>
       </c>
@@ -3020,7 +3044,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="5" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="5" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B5" s="3">
         <v>120</v>
       </c>
@@ -3043,7 +3067,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="6" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="6" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B6" s="3">
         <v>150</v>
       </c>
@@ -3066,7 +3090,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="7" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="7" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B7" s="3">
         <v>180</v>
       </c>
@@ -3089,7 +3113,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="8" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="8" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B8" s="3">
         <v>210</v>
       </c>
@@ -3112,7 +3136,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="9" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="9" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B9" s="2">
         <v>240</v>
       </c>

</xml_diff>

<commit_message>
Finished 74mm measurements, compared with Goda & Suzuki
</commit_message>
<xml_diff>
--- a/Datasets/II Semester 2025/Results - Final Sensors.xlsx
+++ b/Datasets/II Semester 2025/Results - Final Sensors.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Gabu\Documents\GitHub\eWave\Datasets\II Semester 2025\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Daniel Quesada\Documents\GitHub\eWave\Datasets\II Semester 2025\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3480B27B-7A41-45D1-A8F6-4600C372759B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EF89E770-622E-4110-B6A5-97819116F066}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" activeTab="1" xr2:uid="{067E96B3-EB7F-4CEE-B660-BBE446B0B978}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{067E96B3-EB7F-4CEE-B660-BBE446B0B978}"/>
   </bookViews>
   <sheets>
     <sheet name="Results" sheetId="7" r:id="rId1"/>
@@ -49,7 +49,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="28">
   <si>
     <t>Frecuencia (Hz)</t>
   </si>
@@ -118,6 +118,21 @@
   </si>
   <si>
     <t>120b</t>
+  </si>
+  <si>
+    <t>Wavemaker starts to fail</t>
+  </si>
+  <si>
+    <t>Water starts to splash</t>
+  </si>
+  <si>
+    <t>Sensors start to fail significantly</t>
+  </si>
+  <si>
+    <t>Pruebas nivel olas pacifico (74 cm)</t>
+  </si>
+  <si>
+    <t>Pruebas nivel olas pacifico (69 cm)</t>
   </si>
 </sst>
 </file>
@@ -260,7 +275,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="33">
+  <fills count="37">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -438,6 +453,30 @@
       <patternFill patternType="solid">
         <fgColor theme="9" tint="0.39997558519241921"/>
         <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF7C80"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
@@ -621,7 +660,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -638,10 +677,19 @@
     <xf numFmtId="2" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="35" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="2" fontId="0" fillId="36" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -695,6 +743,11 @@
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <mruColors>
+      <color rgb="FFFF7C80"/>
+    </mruColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -1072,15 +1125,15 @@
   <sheetViews>
     <sheetView topLeftCell="A37" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="2" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="2" width="10.6640625" bestFit="1" customWidth="1"/>
     <col min="3" max="10" width="12" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="12.6640625" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="12" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>3</v>
       </c>
@@ -1118,7 +1171,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>10</v>
       </c>
@@ -1156,7 +1209,7 @@
         <v>0.99425987498663038</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>10</v>
       </c>
@@ -1194,7 +1247,7 @@
         <v>1.4319671505134792</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>10</v>
       </c>
@@ -1232,7 +1285,7 @@
         <v>0.66323567967107411</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>10</v>
       </c>
@@ -1270,7 +1323,7 @@
         <v>0.47407032379900588</v>
       </c>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>10</v>
       </c>
@@ -1308,7 +1361,7 @@
         <v>0.5133271289803476</v>
       </c>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>10</v>
       </c>
@@ -1346,7 +1399,7 @@
         <v>0.6844931801537899</v>
       </c>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>12.5</v>
       </c>
@@ -1384,7 +1437,7 @@
         <v>0.87438816285499354</v>
       </c>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>12.5</v>
       </c>
@@ -1422,7 +1475,7 @@
         <v>0.97016321646400394</v>
       </c>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>12.5</v>
       </c>
@@ -1460,7 +1513,7 @@
         <v>0.47393507147560848</v>
       </c>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>12.5</v>
       </c>
@@ -1498,7 +1551,7 @@
         <v>0.40839657223935699</v>
       </c>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>12.5</v>
       </c>
@@ -1536,7 +1589,7 @@
         <v>0.31671180782006297</v>
       </c>
     </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>12.5</v>
       </c>
@@ -1574,7 +1627,7 @@
         <v>3.5125360773263368</v>
       </c>
     </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>15</v>
       </c>
@@ -1612,7 +1665,7 @@
         <v>0.82184594716369452</v>
       </c>
     </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>15</v>
       </c>
@@ -1650,7 +1703,7 @@
         <v>1.6928101718428381</v>
       </c>
     </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>15</v>
       </c>
@@ -1688,7 +1741,7 @@
         <v>0.34912820593784621</v>
       </c>
     </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A17">
         <v>15</v>
       </c>
@@ -1726,7 +1779,7 @@
         <v>1.5829223306549818</v>
       </c>
     </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A18">
         <v>15</v>
       </c>
@@ -1764,7 +1817,7 @@
         <v>0.37239715416958513</v>
       </c>
     </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A19">
         <v>15</v>
       </c>
@@ -1802,7 +1855,7 @@
         <v>0.35146794438723039</v>
       </c>
     </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A20">
         <v>17.5</v>
       </c>
@@ -1840,7 +1893,7 @@
         <v>0.13674233014607934</v>
       </c>
     </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A21">
         <v>17.5</v>
       </c>
@@ -1878,7 +1931,7 @@
         <v>0.20482425169301452</v>
       </c>
     </row>
-    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A22">
         <v>17.5</v>
       </c>
@@ -1916,7 +1969,7 @@
         <v>0.1491713097669646</v>
       </c>
     </row>
-    <row r="23" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A23">
         <v>17.5</v>
       </c>
@@ -1954,7 +2007,7 @@
         <v>0.12632450906248469</v>
       </c>
     </row>
-    <row r="24" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A24">
         <v>17.5</v>
       </c>
@@ -1992,7 +2045,7 @@
         <v>0.17693363368686973</v>
       </c>
     </row>
-    <row r="25" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A25">
         <v>17.5</v>
       </c>
@@ -2030,7 +2083,7 @@
         <v>0.14438635662454116</v>
       </c>
     </row>
-    <row r="26" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A26">
         <v>17.5</v>
       </c>
@@ -2068,7 +2121,7 @@
         <v>0.12280022592880278</v>
       </c>
     </row>
-    <row r="27" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A27">
         <v>17.5</v>
       </c>
@@ -2106,7 +2159,7 @@
         <v>0.12948272793337412</v>
       </c>
     </row>
-    <row r="28" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A28">
         <v>17.5</v>
       </c>
@@ -2144,7 +2197,7 @@
         <v>0.23592606876244379</v>
       </c>
     </row>
-    <row r="29" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A29">
         <v>20</v>
       </c>
@@ -2182,7 +2235,7 @@
         <v>0.11433157394113133</v>
       </c>
     </row>
-    <row r="30" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A30">
         <v>20</v>
       </c>
@@ -2220,7 +2273,7 @@
         <v>3.2960139589624524</v>
       </c>
     </row>
-    <row r="31" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A31">
         <v>20</v>
       </c>
@@ -2258,7 +2311,7 @@
         <v>0.75003182789538847</v>
       </c>
     </row>
-    <row r="32" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A32">
         <v>20</v>
       </c>
@@ -2296,7 +2349,7 @@
         <v>0.14125049962792813</v>
       </c>
     </row>
-    <row r="33" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A33">
         <v>20</v>
       </c>
@@ -2334,7 +2387,7 @@
         <v>0.22937602714105437</v>
       </c>
     </row>
-    <row r="34" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A34">
         <v>20</v>
       </c>
@@ -2372,7 +2425,7 @@
         <v>0.16958907352221608</v>
       </c>
     </row>
-    <row r="35" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A35">
         <v>22.5</v>
       </c>
@@ -2410,7 +2463,7 @@
         <v>3.6844287035645795</v>
       </c>
     </row>
-    <row r="36" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A36">
         <v>22.5</v>
       </c>
@@ -2448,7 +2501,7 @@
         <v>6.7292167108884596E-2</v>
       </c>
     </row>
-    <row r="37" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A37">
         <v>22.5</v>
       </c>
@@ -2486,7 +2539,7 @@
         <v>8.6431833496537824E-2</v>
       </c>
     </row>
-    <row r="38" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A38">
         <v>22.5</v>
       </c>
@@ -2524,7 +2577,7 @@
         <v>0.38469166346338279</v>
       </c>
     </row>
-    <row r="39" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A39">
         <v>22.5</v>
       </c>
@@ -2562,7 +2615,7 @@
         <v>0.15923270965237604</v>
       </c>
     </row>
-    <row r="40" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A40">
         <v>22.5</v>
       </c>
@@ -2600,7 +2653,7 @@
         <v>0.1071048974888421</v>
       </c>
     </row>
-    <row r="41" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A41">
         <v>25</v>
       </c>
@@ -2638,7 +2691,7 @@
         <v>6.2846332685778508E-2</v>
       </c>
     </row>
-    <row r="42" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A42">
         <v>27.5</v>
       </c>
@@ -2676,7 +2729,7 @@
         <v>0.14173594591965136</v>
       </c>
     </row>
-    <row r="43" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A43">
         <v>30</v>
       </c>
@@ -2714,7 +2767,7 @@
         <v>0.49885142281930339</v>
       </c>
     </row>
-    <row r="44" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:12" x14ac:dyDescent="0.3">
       <c r="B44" t="s">
         <v>15</v>
       </c>
@@ -2729,38 +2782,55 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8B065C34-D71F-4F02-8C1B-51E36B9B764A}">
-  <dimension ref="B1:M9"/>
+  <dimension ref="B1:P20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I5" sqref="I5"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="2.7109375" customWidth="1"/>
-    <col min="2" max="3" width="11.140625" customWidth="1"/>
-    <col min="4" max="5" width="9.5703125" bestFit="1" customWidth="1"/>
-    <col min="6" max="8" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="2.6640625" customWidth="1"/>
+    <col min="2" max="3" width="11.109375" customWidth="1"/>
+    <col min="4" max="5" width="9.5546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="8" width="10.5546875" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="26.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="L1" t="s">
+    <row r="1" spans="2:16" x14ac:dyDescent="0.3">
+      <c r="B1" s="11" t="s">
+        <v>26</v>
+      </c>
+      <c r="C1" s="11"/>
+      <c r="D1" s="11"/>
+      <c r="E1" s="11"/>
+      <c r="F1" s="11"/>
+      <c r="G1" s="11"/>
+      <c r="H1" s="11"/>
+      <c r="I1" s="11"/>
+      <c r="J1" s="11"/>
+      <c r="K1" s="11"/>
+      <c r="L1" s="11"/>
+      <c r="M1" s="11"/>
+      <c r="N1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B2" s="3"/>
-      <c r="C2" s="6" t="s">
+      <c r="C2" s="12" t="s">
         <v>0</v>
       </c>
-      <c r="D2" s="6"/>
-      <c r="E2" s="6"/>
-      <c r="F2" s="6"/>
-      <c r="G2" s="6"/>
-      <c r="H2" s="6"/>
-      <c r="I2" s="6"/>
-    </row>
-    <row r="3" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="D2" s="12"/>
+      <c r="E2" s="12"/>
+      <c r="F2" s="12"/>
+      <c r="G2" s="12"/>
+      <c r="H2" s="12"/>
+      <c r="I2" s="12"/>
+      <c r="J2" s="12"/>
+      <c r="K2" s="12"/>
+      <c r="L2" s="12"/>
+      <c r="M2" s="12"/>
+    </row>
+    <row r="3" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B3" s="1" t="s">
         <v>1</v>
       </c>
@@ -2798,7 +2868,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="4" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B4" s="3">
         <v>90</v>
       </c>
@@ -2835,8 +2905,11 @@
       <c r="M4" s="4">
         <v>107.52</v>
       </c>
-    </row>
-    <row r="5" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="P4" s="7" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="5" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B5" s="3">
         <v>120</v>
       </c>
@@ -2858,10 +2931,23 @@
       <c r="H5" s="4">
         <v>61.142962025316457</v>
       </c>
-      <c r="I5" s="4"/>
-      <c r="J5" s="4"/>
-    </row>
-    <row r="6" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="I5" s="4">
+        <v>94.31</v>
+      </c>
+      <c r="J5" s="4">
+        <v>118.25</v>
+      </c>
+      <c r="K5" s="4">
+        <v>84.42</v>
+      </c>
+      <c r="L5" s="7">
+        <v>108.22</v>
+      </c>
+      <c r="P5" s="9" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="6" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B6" s="3">
         <v>150</v>
       </c>
@@ -2883,10 +2969,17 @@
       <c r="H6" s="4">
         <v>75.606683544303792</v>
       </c>
-      <c r="I6" s="4"/>
-      <c r="J6" s="4"/>
-    </row>
-    <row r="7" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="I6" s="4">
+        <v>110.92</v>
+      </c>
+      <c r="J6" s="7">
+        <v>147.86000000000001</v>
+      </c>
+      <c r="P6" s="8" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="7" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B7" s="3">
         <v>180</v>
       </c>
@@ -2908,10 +3001,12 @@
       <c r="H7" s="4">
         <v>87.952253164556964</v>
       </c>
-      <c r="I7" s="4"/>
+      <c r="I7" s="7">
+        <v>134.02000000000001</v>
+      </c>
       <c r="J7" s="4"/>
     </row>
-    <row r="8" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B8" s="3">
         <v>210</v>
       </c>
@@ -2933,10 +3028,12 @@
       <c r="H8" s="4">
         <v>99.898253164556962</v>
       </c>
-      <c r="I8" s="4"/>
+      <c r="I8" s="10">
+        <v>150.96</v>
+      </c>
       <c r="J8" s="4"/>
     </row>
-    <row r="9" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B9" s="2">
         <v>240</v>
       </c>
@@ -2964,9 +3061,265 @@
       <c r="L9" s="5"/>
       <c r="M9" s="5"/>
     </row>
+    <row r="12" spans="2:16" x14ac:dyDescent="0.3">
+      <c r="B12" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="C12" s="11"/>
+      <c r="D12" s="11"/>
+      <c r="E12" s="11"/>
+      <c r="F12" s="11"/>
+      <c r="G12" s="11"/>
+      <c r="H12" s="11"/>
+      <c r="I12" s="11"/>
+      <c r="J12" s="11"/>
+      <c r="K12" s="11"/>
+      <c r="L12" s="11"/>
+      <c r="M12" s="11"/>
+    </row>
+    <row r="13" spans="2:16" x14ac:dyDescent="0.3">
+      <c r="C13" s="12" t="s">
+        <v>0</v>
+      </c>
+      <c r="D13" s="12"/>
+      <c r="E13" s="12"/>
+      <c r="F13" s="12"/>
+      <c r="G13" s="12"/>
+      <c r="H13" s="12"/>
+      <c r="I13" s="12"/>
+      <c r="J13" s="12"/>
+      <c r="K13" s="12"/>
+      <c r="L13" s="12"/>
+      <c r="M13" s="12"/>
+    </row>
+    <row r="14" spans="2:16" x14ac:dyDescent="0.3">
+      <c r="B14" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C14" s="1">
+        <v>10</v>
+      </c>
+      <c r="D14" s="1">
+        <v>12.5</v>
+      </c>
+      <c r="E14" s="1">
+        <v>15</v>
+      </c>
+      <c r="F14" s="1">
+        <v>17.5</v>
+      </c>
+      <c r="G14" s="1">
+        <v>20</v>
+      </c>
+      <c r="H14" s="1">
+        <v>22.5</v>
+      </c>
+      <c r="I14" s="1">
+        <v>25</v>
+      </c>
+      <c r="J14" s="1">
+        <v>27.5</v>
+      </c>
+      <c r="K14" s="1">
+        <v>30</v>
+      </c>
+      <c r="L14" s="1">
+        <v>32.5</v>
+      </c>
+      <c r="M14" s="1">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="15" spans="2:16" x14ac:dyDescent="0.3">
+      <c r="B15" s="3">
+        <v>90</v>
+      </c>
+      <c r="C15" s="4">
+        <v>25.943822784810127</v>
+      </c>
+      <c r="D15" s="4">
+        <v>17.605999999999998</v>
+      </c>
+      <c r="E15" s="4">
+        <v>41.455898734177197</v>
+      </c>
+      <c r="F15" s="4">
+        <v>48.408075949367088</v>
+      </c>
+      <c r="G15" s="4">
+        <v>61.213670886075953</v>
+      </c>
+      <c r="H15" s="4">
+        <v>49.597924050632912</v>
+      </c>
+      <c r="I15" s="4">
+        <v>73.941189873417727</v>
+      </c>
+      <c r="J15" s="4">
+        <v>101.45691139240506</v>
+      </c>
+      <c r="K15" s="4">
+        <v>65.3</v>
+      </c>
+      <c r="L15" s="4">
+        <v>84.49</v>
+      </c>
+      <c r="M15" s="4">
+        <v>107.52</v>
+      </c>
+    </row>
+    <row r="16" spans="2:16" x14ac:dyDescent="0.3">
+      <c r="B16" s="3">
+        <v>120</v>
+      </c>
+      <c r="C16" s="4">
+        <v>30.072126582278482</v>
+      </c>
+      <c r="D16" s="4">
+        <v>22.845848101265823</v>
+      </c>
+      <c r="E16" s="4">
+        <v>54.199518987341769</v>
+      </c>
+      <c r="F16" s="4">
+        <v>58.283037974683545</v>
+      </c>
+      <c r="G16" s="4">
+        <v>73.502784810126585</v>
+      </c>
+      <c r="H16" s="4">
+        <v>61.142962025316457</v>
+      </c>
+      <c r="I16" s="4">
+        <v>94.31</v>
+      </c>
+      <c r="J16" s="4">
+        <v>118.25</v>
+      </c>
+      <c r="K16" s="4">
+        <v>84.42</v>
+      </c>
+      <c r="L16" s="7">
+        <v>108.22</v>
+      </c>
+    </row>
+    <row r="17" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="B17" s="3">
+        <v>150</v>
+      </c>
+      <c r="C17" s="4">
+        <v>34.224962025316458</v>
+      </c>
+      <c r="D17" s="4">
+        <v>26.487392405063289</v>
+      </c>
+      <c r="E17" s="4">
+        <v>59.902506329113898</v>
+      </c>
+      <c r="F17" s="4">
+        <v>70.313291139240505</v>
+      </c>
+      <c r="G17" s="4">
+        <v>85.81311392405064</v>
+      </c>
+      <c r="H17" s="4">
+        <v>75.606683544303792</v>
+      </c>
+      <c r="I17" s="4">
+        <v>110.92</v>
+      </c>
+      <c r="J17" s="7">
+        <v>147.86000000000001</v>
+      </c>
+    </row>
+    <row r="18" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="B18" s="3">
+        <v>180</v>
+      </c>
+      <c r="C18" s="4">
+        <v>38.721620253164559</v>
+      </c>
+      <c r="D18" s="4">
+        <v>31.635696202531648</v>
+      </c>
+      <c r="E18" s="4">
+        <v>74.032506329113929</v>
+      </c>
+      <c r="F18" s="4">
+        <v>82.847240506329115</v>
+      </c>
+      <c r="G18" s="4">
+        <v>98.923815789473679</v>
+      </c>
+      <c r="H18" s="4">
+        <v>87.952253164556964</v>
+      </c>
+      <c r="I18" s="7">
+        <v>134.02000000000001</v>
+      </c>
+      <c r="J18" s="4"/>
+    </row>
+    <row r="19" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="B19" s="3">
+        <v>210</v>
+      </c>
+      <c r="C19" s="4">
+        <v>40.373797468354432</v>
+      </c>
+      <c r="D19" s="4">
+        <v>34.37341772151899</v>
+      </c>
+      <c r="E19" s="4">
+        <v>79.921772151898693</v>
+      </c>
+      <c r="F19" s="4">
+        <v>94.448227848101268</v>
+      </c>
+      <c r="G19" s="4">
+        <v>114.66673417721519</v>
+      </c>
+      <c r="H19" s="4">
+        <v>99.898253164556962</v>
+      </c>
+      <c r="I19" s="10">
+        <v>150.96</v>
+      </c>
+      <c r="J19" s="4"/>
+    </row>
+    <row r="20" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="B20" s="2">
+        <v>240</v>
+      </c>
+      <c r="C20" s="5">
+        <v>44.132936708860761</v>
+      </c>
+      <c r="D20" s="5">
+        <v>40.320101265822785</v>
+      </c>
+      <c r="E20" s="5">
+        <v>89.431051282051286</v>
+      </c>
+      <c r="F20" s="5">
+        <v>107.3167341772152</v>
+      </c>
+      <c r="G20" s="5">
+        <v>131.08458227848101</v>
+      </c>
+      <c r="H20" s="5">
+        <v>126.13407594936709</v>
+      </c>
+      <c r="I20" s="5"/>
+      <c r="J20" s="5"/>
+      <c r="K20" s="5"/>
+      <c r="L20" s="5"/>
+      <c r="M20" s="5"/>
+    </row>
   </sheetData>
-  <mergeCells count="1">
-    <mergeCell ref="C2:I2"/>
+  <mergeCells count="4">
+    <mergeCell ref="B1:M1"/>
+    <mergeCell ref="B12:M12"/>
+    <mergeCell ref="C2:M2"/>
+    <mergeCell ref="C13:M13"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -2978,27 +3331,27 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="2.7109375" customWidth="1"/>
-    <col min="2" max="3" width="11.140625" customWidth="1"/>
+    <col min="1" max="1" width="2.6640625" customWidth="1"/>
+    <col min="2" max="3" width="11.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B2" s="3"/>
-      <c r="C2" s="7" t="s">
+      <c r="C2" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="D2" s="7"/>
-      <c r="E2" s="7"/>
-      <c r="F2" s="7"/>
-      <c r="G2" s="7"/>
-      <c r="H2" s="7"/>
+      <c r="D2" s="6"/>
+      <c r="E2" s="6"/>
+      <c r="F2" s="6"/>
+      <c r="G2" s="6"/>
+      <c r="H2" s="6"/>
       <c r="J2" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B3" s="1" t="s">
         <v>1</v>
       </c>
@@ -3021,7 +3374,7 @@
         <v>22.5</v>
       </c>
     </row>
-    <row r="4" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B4" s="3">
         <v>90</v>
       </c>
@@ -3044,7 +3397,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="5" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B5" s="3">
         <v>120</v>
       </c>
@@ -3067,7 +3420,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="6" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B6" s="3">
         <v>150</v>
       </c>
@@ -3090,7 +3443,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="7" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B7" s="3">
         <v>180</v>
       </c>
@@ -3113,7 +3466,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="8" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B8" s="3">
         <v>210</v>
       </c>
@@ -3136,7 +3489,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="9" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B9" s="2">
         <v>240</v>
       </c>

</xml_diff>